<commit_message>
some Fix and video link
</commit_message>
<xml_diff>
--- a/resultData/Носки.xlsx
+++ b/resultData/Носки.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\clouds\Dropbox\programming\UTM\resultData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B8A86-DF1E-439D-B459-9EFC86B48FB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89060A6F-A0D3-4EAD-A9BC-E3B6671A0340}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,15 +85,45 @@
     <t>Количество в упаковке</t>
   </si>
   <si>
+    <t>933141</t>
+  </si>
+  <si>
+    <t>Носки мужские х/б черные р.40 ФКУ ИК-1 ГУФСИН РОССИИ ПО ЧЕЛЯБИНСКОЙ ОБЛАСТИ Россия</t>
+  </si>
+  <si>
+    <t>Носки</t>
+  </si>
+  <si>
+    <t>14.31.10</t>
+  </si>
+  <si>
+    <t>р.40</t>
+  </si>
+  <si>
+    <t>ФКУ ИК-1 ГУФСИН РОССИИ ПО ЧЕЛЯБИНСКОЙ ОБЛАСТИ</t>
+  </si>
+  <si>
+    <t>мужские</t>
+  </si>
+  <si>
+    <t>черные</t>
+  </si>
+  <si>
+    <t>1,0274007795e+12</t>
+  </si>
+  <si>
+    <t>хлопчатобумажные</t>
+  </si>
+  <si>
+    <t>Россия</t>
+  </si>
+  <si>
     <t>144581</t>
   </si>
   <si>
     <t>Носки спортивные Forward трикотаж, 85% хлопок , 12% ПЭ, 3% эластан черный/белый/серый 3 пары</t>
   </si>
   <si>
-    <t>14.31.10</t>
-  </si>
-  <si>
     <t>спортивные</t>
   </si>
   <si>
@@ -109,36 +139,6 @@
     <t>3 пары</t>
   </si>
   <si>
-    <t>933141</t>
-  </si>
-  <si>
-    <t>Носки мужские х/б черные р.40 ФКУ ИК-1 ГУФСИН РОССИИ ПО ЧЕЛЯБИНСКОЙ ОБЛАСТИ Россия</t>
-  </si>
-  <si>
-    <t>Носки</t>
-  </si>
-  <si>
-    <t>р.40</t>
-  </si>
-  <si>
-    <t>ФКУ ИК-1 ГУФСИН РОССИИ ПО ЧЕЛЯБИНСКОЙ ОБЛАСТИ</t>
-  </si>
-  <si>
-    <t>мужские</t>
-  </si>
-  <si>
-    <t>черные</t>
-  </si>
-  <si>
-    <t>1,0274007795e+12</t>
-  </si>
-  <si>
-    <t>хлопчатобумажные</t>
-  </si>
-  <si>
-    <t>Россия</t>
-  </si>
-  <si>
     <t>943460</t>
   </si>
   <si>
@@ -208,6 +208,18 @@
     <t xml:space="preserve">Butterfly </t>
   </si>
   <si>
+    <t>54124</t>
+  </si>
+  <si>
+    <t>Носки нагольные для особого пояса ТИС натуральная овчина мужские</t>
+  </si>
+  <si>
+    <t>нагольные для особого пояса ТИС</t>
+  </si>
+  <si>
+    <t>натуральная овчина</t>
+  </si>
+  <si>
     <t>115169</t>
   </si>
   <si>
@@ -220,18 +232,6 @@
     <t>Asics</t>
   </si>
   <si>
-    <t>54124</t>
-  </si>
-  <si>
-    <t>Носки нагольные для особого пояса ТИС натуральная овчина мужские</t>
-  </si>
-  <si>
-    <t>нагольные для особого пояса ТИС</t>
-  </si>
-  <si>
-    <t>натуральная овчина</t>
-  </si>
-  <si>
     <t>967697</t>
   </si>
   <si>
@@ -277,6 +277,15 @@
     <t>р.29</t>
   </si>
   <si>
+    <t>663133</t>
+  </si>
+  <si>
+    <t>Носки М -01 хлопок</t>
+  </si>
+  <si>
+    <t>М -01</t>
+  </si>
+  <si>
     <t>663426</t>
   </si>
   <si>
@@ -284,15 +293,6 @@
   </si>
   <si>
     <t>170968</t>
-  </si>
-  <si>
-    <t>663133</t>
-  </si>
-  <si>
-    <t>Носки М -01 хлопок</t>
-  </si>
-  <si>
-    <t>М -01</t>
   </si>
   <si>
     <t>4014</t>
@@ -647,7 +647,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +807,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>15676.42333165164</v>
+        <v>18170.305223310272</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -816,68 +816,68 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>15405.203259841701</v>
+        <v>17036.43680888748</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
         <v>34</v>
       </c>
       <c r="L5" t="s">
         <v>35</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>13021.626157734419</v>
+        <v>15673.29519179395</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -886,10 +886,10 @@
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
         <v>41</v>
@@ -901,7 +901,7 @@
         <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
         <v>44</v>
@@ -913,12 +913,12 @@
         <v>46</v>
       </c>
       <c r="Q6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>12396.13437305337</v>
+        <v>14964.307083964441</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -927,10 +927,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
         <v>41</v>
@@ -942,24 +942,24 @@
         <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M7" t="s">
         <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="O7" t="s">
         <v>46</v>
       </c>
       <c r="Q7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12087.90436775018</v>
+        <v>13276.45486626453</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -971,7 +971,7 @@
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L8" t="s">
         <v>52</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9828.4460936020405</v>
+        <v>10891.60069280218</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -1000,7 +1000,7 @@
         <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8765.265602254407</v>
+        <v>10436.64239921783</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
@@ -1026,21 +1026,21 @@
         <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
-      </c>
-      <c r="O10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7873.1782979759464</v>
+        <v>9803.0585959172295</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
@@ -1052,21 +1052,21 @@
         <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" t="s">
         <v>68</v>
       </c>
-      <c r="K11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5941.8466886397346</v>
+        <v>6120.9798697324213</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -1075,10 +1075,10 @@
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
         <v>72</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4922.6677044455382</v>
+        <v>5344.7997979502898</v>
       </c>
       <c r="B13" t="s">
         <v>75</v>
@@ -1104,7 +1104,7 @@
         <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
         <v>77</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4922.6677044455382</v>
+        <v>5344.7997979502898</v>
       </c>
       <c r="B14" t="s">
         <v>79</v>
@@ -1130,7 +1130,7 @@
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H14" t="s">
         <v>81</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4922.6677044455382</v>
+        <v>5344.7997979502898</v>
       </c>
       <c r="B15" t="s">
         <v>82</v>
@@ -1156,7 +1156,7 @@
         <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
         <v>84</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3948.1305501768202</v>
+        <v>4185.88296406268</v>
       </c>
       <c r="B16" t="s">
         <v>85</v>
@@ -1182,18 +1182,18 @@
         <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
       </c>
       <c r="N16" t="s">
-        <v>73</v>
-      </c>
-      <c r="R16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3908.99845135536</v>
+        <v>4182.3843781768037</v>
       </c>
       <c r="B17" t="s">
         <v>88</v>
@@ -1205,18 +1205,18 @@
         <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>73</v>
+      </c>
+      <c r="R17" t="s">
         <v>90</v>
       </c>
-      <c r="N17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1876.4753540431529</v>
+        <v>2126.9643234885102</v>
       </c>
       <c r="B18" t="s">
         <v>91</v>
@@ -1228,15 +1228,15 @@
         <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>625.49178468105094</v>
+        <v>708.98810782950318</v>
       </c>
       <c r="B19" t="s">
         <v>93</v>
@@ -1248,14 +1248,14 @@
         <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N19" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:S2">
+  <conditionalFormatting sqref="A1:XFD2">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>